<commit_message>
"fix bug edit data pemilih for admin role"
</commit_message>
<xml_diff>
--- a/rekapan.xlsx
+++ b/rekapan.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="138">
   <si>
     <t>ALAT KERJA BAWASLU KABUPATEN/KOTA</t>
   </si>
@@ -77,19 +77,28 @@
     <t>Nama Pengawas</t>
   </si>
   <si>
-    <t>Pengawas 1</t>
+    <t>Leon</t>
   </si>
   <si>
     <t>Jabatan Pengawas Pemilu</t>
   </si>
   <si>
+    <t>Panwascam</t>
+  </si>
+  <si>
     <t>No HP</t>
   </si>
   <si>
     <t>Kab/Kota</t>
   </si>
   <si>
+    <t>Kupang</t>
+  </si>
+  <si>
     <t>Provinsi</t>
+  </si>
+  <si>
+    <t>Nusa Tenggara Timur</t>
   </si>
   <si>
     <r>
@@ -400,9 +409,6 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Kupang</t>
-  </si>
-  <si>
     <t>1965-12-05</t>
   </si>
   <si>
@@ -428,9 +434,6 @@
   </si>
   <si>
     <t>Kupang Barat</t>
-  </si>
-  <si>
-    <t>Nusa Tenggara Timur</t>
   </si>
   <si>
     <t>Naibila Nibala</t>
@@ -1569,18 +1572,20 @@
         <v>6</v>
       </c>
       <c r="B8" s="26"/>
-      <c r="C8" s="25"/>
+      <c r="C8" s="25" t="s">
+        <v>7</v>
+      </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
     </row>
     <row r="9" spans="1:6" customHeight="1" ht="24">
       <c r="A9" s="26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="25">
-        <v>0</v>
+        <v>2147483647</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -1588,20 +1593,24 @@
     </row>
     <row r="10" spans="1:6" customHeight="1" ht="24">
       <c r="A10" s="26" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="26"/>
-      <c r="C10" s="25"/>
+      <c r="C10" s="25" t="s">
+        <v>10</v>
+      </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
     </row>
     <row r="11" spans="1:6" customHeight="1" ht="24">
       <c r="A11" s="26" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" s="26"/>
-      <c r="C11" s="25"/>
+      <c r="C11" s="25" t="s">
+        <v>12</v>
+      </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
@@ -1611,7 +1620,7 @@
     </row>
     <row r="13" spans="1:6" customHeight="1" ht="15.75">
       <c r="A13" s="24" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
@@ -1620,19 +1629,19 @@
     </row>
     <row r="14" spans="1:6" customHeight="1" ht="45.75">
       <c r="A14" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:6" customHeight="1" ht="15.75">
@@ -1640,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1651,7 +1660,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1662,7 +1671,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -1766,7 +1775,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1774,44 +1783,44 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
@@ -1826,40 +1835,40 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
       <c r="G4" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>8</v>
-      </c>
       <c r="T4" s="30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:20" customHeight="1" ht="18">
@@ -1880,7 +1889,7 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
@@ -2098,7 +2107,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2106,44 +2115,44 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
@@ -2158,40 +2167,40 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
       <c r="G4" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>8</v>
-      </c>
       <c r="T4" s="30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:20" customHeight="1" ht="18">
@@ -2212,7 +2221,7 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
@@ -2430,7 +2439,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2438,44 +2447,44 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
@@ -2494,34 +2503,34 @@
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>8</v>
-      </c>
       <c r="T4" s="30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:20" customHeight="1" ht="18">
@@ -2542,7 +2551,7 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
@@ -2761,7 +2770,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2769,44 +2778,44 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
@@ -2821,40 +2830,40 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
       <c r="G4" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>8</v>
-      </c>
       <c r="T4" s="30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:20" customHeight="1" ht="18">
@@ -2875,7 +2884,7 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
@@ -2883,126 +2892,126 @@
     </row>
     <row r="6" spans="1:20" customHeight="1" ht="18">
       <c r="A6" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B6" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K6" s="21">
         <v>2</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="P6" s="21">
         <v>1</v>
       </c>
       <c r="Q6" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S6" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B7" s="11">
         <v>0</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K7" s="11">
         <v>14</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="P7" s="11">
         <v>10</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -3217,7 +3226,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -3225,44 +3234,44 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
@@ -3277,40 +3286,40 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
       <c r="G4" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>8</v>
-      </c>
       <c r="T4" s="30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:20" customHeight="1" ht="18">
@@ -3331,7 +3340,7 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
@@ -3549,7 +3558,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -3557,44 +3566,44 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
@@ -3609,40 +3618,40 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
       <c r="G4" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>8</v>
-      </c>
       <c r="T4" s="30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:20" customHeight="1" ht="18">
@@ -3663,7 +3672,7 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
@@ -3671,64 +3680,64 @@
     </row>
     <row r="6" spans="1:20" customHeight="1" ht="18">
       <c r="A6" s="21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B6" s="21">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K6" s="21">
         <v>2</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="P6" s="21">
         <v>1</v>
       </c>
       <c r="Q6" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S6" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -3943,7 +3952,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -3951,44 +3960,44 @@
     </row>
     <row r="3" spans="1:20" customHeight="1" ht="15.75">
       <c r="A3" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
@@ -4003,40 +4012,40 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
       <c r="G4" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>8</v>
-      </c>
       <c r="T4" s="30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:20" customHeight="1" ht="18">
@@ -4057,7 +4066,7 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
@@ -4065,126 +4074,126 @@
     </row>
     <row r="6" spans="1:20" customHeight="1" ht="18">
       <c r="A6" s="21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B6" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K6" s="21">
         <v>2</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="P6" s="21">
         <v>1</v>
       </c>
       <c r="Q6" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S6" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B7" s="11">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K7" s="11">
         <v>1</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="P7" s="11">
         <v>2</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -4400,7 +4409,7 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -4408,57 +4417,57 @@
     </row>
     <row r="3" spans="1:23" customHeight="1" ht="35.25">
       <c r="A3" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29"/>
       <c r="Q3" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="R3" s="29"/>
       <c r="S3" s="29"/>
       <c r="T3" s="29"/>
       <c r="U3" s="29"/>
       <c r="V3" s="29" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="W3" s="29" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:23" customHeight="1" ht="36">
@@ -4469,171 +4478,171 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
       <c r="G4" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
       <c r="L4" s="19" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="M4" s="19" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="N4" s="19" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="S4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="T4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="R4" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="S4" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="T4" s="19" t="s">
-        <v>8</v>
-      </c>
       <c r="U4" s="19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="V4" s="29"/>
       <c r="W4" s="29"/>
     </row>
     <row r="5" spans="1:23" customHeight="1" ht="18">
       <c r="A5" s="21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B5" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K5" s="21"/>
       <c r="L5" s="21">
         <v>2</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="Q5" s="21">
         <v>1</v>
       </c>
       <c r="R5" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S5" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="T5" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="U5" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="V5" s="21"/>
       <c r="W5" s="21"/>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B6" s="11">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11">
         <v>1</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="Q6" s="11">
         <v>2</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
@@ -4872,18 +4881,18 @@
   <sheetData>
     <row r="1" spans="1:12" customHeight="1" ht="15.75">
       <c r="A1" s="7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="27" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
@@ -4899,34 +4908,34 @@
       <c r="A3" s="27"/>
       <c r="B3" s="27"/>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4934,7 +4943,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4" s="10">
         <v>1</v>
@@ -4972,7 +4981,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="11">
         <v>0</v>
@@ -5010,7 +5019,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C6" s="11">
         <v>0</v>
@@ -5181,18 +5190,18 @@
   <sheetData>
     <row r="1" spans="1:9" customHeight="1" ht="31.5">
       <c r="A1" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" customHeight="1" ht="53.25">
       <c r="A2" s="15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -5206,7 +5215,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" s="15">
         <v>0</v>
@@ -5223,7 +5232,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" s="25">
         <v>0</v>
@@ -5240,7 +5249,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5" s="25">
         <v>0</v>
@@ -5371,18 +5380,18 @@
   <sheetData>
     <row r="1" spans="1:3" customHeight="1" ht="30.75">
       <c r="A1" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" customHeight="1" ht="15.75">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" customHeight="1" ht="15.75">
@@ -5390,7 +5399,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" s="5">
         <v>2</v>
@@ -5401,7 +5410,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5">
         <v>2</v>
@@ -5412,7 +5421,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -5453,7 +5462,7 @@
   <sheetData>
     <row r="1" spans="1:3" customHeight="1" ht="15.75">
       <c r="A1" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" customHeight="1" ht="15.75">
@@ -5461,13 +5470,13 @@
     </row>
     <row r="3" spans="1:3" customHeight="1" ht="47.25">
       <c r="A3" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" customHeight="1" ht="15.75">
@@ -5515,51 +5524,51 @@
   <sheetData>
     <row r="1" spans="1:18" customHeight="1" ht="15.75">
       <c r="A1" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="29" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="O2" s="29"/>
       <c r="P2" s="29"/>
@@ -5578,24 +5587,24 @@
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
       <c r="K3" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="19" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="P3" s="19" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:18" customHeight="1" ht="18">
@@ -5606,52 +5615,52 @@
         <v>9879879879</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F4" s="21">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M4" s="21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N4" s="21">
         <v>2</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q4" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="R4" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -5662,37 +5671,37 @@
         <v>5474574734</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F5" s="11">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
@@ -5708,52 +5717,52 @@
         <v>5371062403050002</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F6" s="11">
         <v>0</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="N6" s="11">
         <v>16</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -5764,52 +5773,52 @@
         <v>5371062403050002</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F7" s="11">
         <v>0</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="N7" s="11">
         <v>1</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -6003,49 +6012,49 @@
   <sheetData>
     <row r="1" spans="1:20" customHeight="1" ht="15.75">
       <c r="A1" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
       <c r="O2" s="29"/>
       <c r="P2" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q2" s="29"/>
       <c r="R2" s="29"/>
@@ -6060,40 +6069,40 @@
       <c r="E3" s="29"/>
       <c r="F3" s="29"/>
       <c r="G3" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H3" s="29"/>
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
       <c r="K3" s="30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M3" s="30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N3" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O3" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="S3" s="30" t="s">
-        <v>8</v>
-      </c>
       <c r="T3" s="30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:20" customHeight="1" ht="18">
@@ -6114,7 +6123,7 @@
       <c r="O4" s="30"/>
       <c r="P4" s="30"/>
       <c r="Q4" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R4" s="30"/>
       <c r="S4" s="30"/>
@@ -6122,64 +6131,64 @@
     </row>
     <row r="5" spans="1:20" customHeight="1" ht="18">
       <c r="A5" s="21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B5" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K5" s="21">
         <v>2</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="P5" s="21">
         <v>2</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R5" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="S5" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="T5" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -6394,7 +6403,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -6402,44 +6411,44 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
@@ -6454,40 +6463,40 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
       <c r="G4" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>8</v>
-      </c>
       <c r="T4" s="30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:20" customHeight="1" ht="18">
@@ -6508,7 +6517,7 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
@@ -6516,64 +6525,64 @@
     </row>
     <row r="6" spans="1:20" customHeight="1" ht="18">
       <c r="A6" s="21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B6" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K6" s="21">
         <v>1</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="P6" s="21">
         <v>2</v>
       </c>
       <c r="Q6" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="S6" s="21" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -6788,7 +6797,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -6796,44 +6805,44 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
@@ -6848,40 +6857,40 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
       <c r="G4" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>8</v>
-      </c>
       <c r="T4" s="30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:20" customHeight="1" ht="18">
@@ -6902,7 +6911,7 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>

</xml_diff>